<commit_message>
Se sube los primeros 3 puntos del escrito
</commit_message>
<xml_diff>
--- a/TP3/outputs/reports.xlsx
+++ b/TP3/outputs/reports.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="113" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="52">
   <si>
     <t>decipcf</t>
   </si>
@@ -53,12 +53,138 @@
   </si>
   <si>
     <t>shr_ipcf</t>
+  </si>
+  <si>
+    <t>decipcf</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>media_c</t>
+  </si>
+  <si>
+    <t>shr_c</t>
+  </si>
+  <si>
+    <t>deccpcf</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>media_c</t>
+  </si>
+  <si>
+    <t>shr_c</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>deccpcf</t>
+  </si>
+  <si>
+    <t>shr_cpcf</t>
+  </si>
+  <si>
+    <t>shr_cigar</t>
+  </si>
+  <si>
+    <t>presion</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>decipcf</t>
+  </si>
+  <si>
+    <t>shr_ipcf</t>
+  </si>
+  <si>
+    <t>shr_cigar</t>
+  </si>
+  <si>
+    <t>presion</t>
+  </si>
+  <si>
+    <t>decipcf</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>media_c</t>
+  </si>
+  <si>
+    <t>shr_c</t>
+  </si>
+  <si>
+    <t>deccpcf</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>media_c</t>
+  </si>
+  <si>
+    <t>shr_c</t>
+  </si>
+  <si>
+    <t>decipcf</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>media_c</t>
+  </si>
+  <si>
+    <t>shr_c</t>
+  </si>
+  <si>
+    <t>deccpcf</t>
+  </si>
+  <si>
+    <t>table1</t>
+  </si>
+  <si>
+    <t>table2</t>
+  </si>
+  <si>
+    <t>media_c</t>
+  </si>
+  <si>
+    <t>shr_c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -444,29 +570,29 @@
       <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.140625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -483,7 +609,7 @@
         <v>1.7653779983520508</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -500,7 +626,7 @@
         <v>3.0953712463378906</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -517,7 +643,7 @@
         <v>4.1890287399291992</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -534,7 +660,7 @@
         <v>5.3398613929748535</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -551,7 +677,7 @@
         <v>6.5982551574707031</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -568,7 +694,7 @@
         <v>7.9534897804260254</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -585,7 +711,7 @@
         <v>9.680912971496582</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -593,7 +719,7 @@
         <v>4034039</v>
       </c>
       <c r="C9" s="1">
-        <v>49454936419.249024</v>
+        <v>49454936419.249023</v>
       </c>
       <c r="D9" s="1">
         <v>12259.4091796875</v>
@@ -602,7 +728,7 @@
         <v>12.177967071533203</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -619,7 +745,7 @@
         <v>16.61625862121582</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -651,19 +777,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -850,22 +976,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
@@ -1100,22 +1226,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -1201,7 +1327,7 @@
         <v>21685270102.393066</v>
       </c>
       <c r="B6" s="1">
-        <v>264037994.53869248</v>
+        <v>264037994.53869247</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1278,7 +1404,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>49454936419.249024</v>
+        <v>49454936419.249023</v>
       </c>
       <c r="B10" s="1">
         <v>313905283.78755951</v>
@@ -1301,7 +1427,7 @@
         <v>67478913183.34375</v>
       </c>
       <c r="B11" s="1">
-        <v>357180518.05638886</v>
+        <v>357180518.05638885</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>

</xml_diff>